<commit_message>
FINALLY CLEANED THE DATA
</commit_message>
<xml_diff>
--- a/fies-lfs_2021_metadata(dictionary).xlsx
+++ b/fies-lfs_2021_metadata(dictionary).xlsx
@@ -1,36 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KRISTY\Desktop\FIES-LFS Merged\2021\Updated FIES-LFS 2021\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JeeYo\Documents\SY. 2024-2025\First Sem\Data Warehouse\PHL-PSA-FIES-LFS-2021-PUF\dw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{69951394-6580-465C-854A-DC64DC569803}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EF9B742-C8A1-4A44-9551-BC8483BF8D68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2205" yWindow="225" windowWidth="15090" windowHeight="14955" xr2:uid="{192F0927-2894-4714-96D2-7EDB43FBAFDE}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{192F0927-2894-4714-96D2-7EDB43FBAFDE}"/>
   </bookViews>
   <sheets>
     <sheet name="fies-lfs_2021_dictionary" sheetId="1" r:id="rId1"/>
     <sheet name="fies-lfs_2021_valueset" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -15691,12 +15680,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -15711,9 +15706,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -16028,13 +16025,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5577198-A831-413B-93A2-A561A8988054}">
-  <dimension ref="A1:F157"/>
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:G157"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M27" sqref="M27"/>
+    <sheetView topLeftCell="A124" workbookViewId="0">
+      <selection activeCell="E170" sqref="E170"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="58.140625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -16053,26 +16054,26 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E3" t="s">
+      <c r="E3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E4" t="s">
+      <c r="E4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E5" t="s">
+      <c r="E5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="2" t="s">
         <v>9</v>
       </c>
     </row>
@@ -16909,18 +16910,18 @@
       </c>
     </row>
     <row r="110" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="E110" t="s">
+      <c r="E110" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="F110" t="s">
+      <c r="F110" s="2" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="111" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="E111" t="s">
+      <c r="E111" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="F111" t="s">
+      <c r="F111" s="2" t="s">
         <v>220</v>
       </c>
     </row>
@@ -16933,34 +16934,34 @@
       </c>
     </row>
     <row r="113" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E113" t="s">
+      <c r="E113" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="F113" t="s">
+      <c r="F113" s="2" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="114" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E114" t="s">
+      <c r="E114" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="F114" t="s">
+      <c r="F114" s="2" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="115" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E115" t="s">
+      <c r="E115" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="F115" t="s">
+      <c r="F115" s="2" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="116" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E116" t="s">
+      <c r="E116" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="F116" t="s">
+      <c r="F116" s="2" t="s">
         <v>230</v>
       </c>
     </row>
@@ -16989,10 +16990,10 @@
       </c>
     </row>
     <row r="120" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E120" t="s">
+      <c r="E120" s="3" t="s">
         <v>237</v>
       </c>
-      <c r="F120" t="s">
+      <c r="F120" s="3" t="s">
         <v>238</v>
       </c>
     </row>
@@ -17021,10 +17022,10 @@
       </c>
     </row>
     <row r="124" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E124" t="s">
+      <c r="E124" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="F124" t="s">
+      <c r="F124" s="2" t="s">
         <v>246</v>
       </c>
     </row>
@@ -17053,22 +17054,23 @@
       </c>
     </row>
     <row r="128" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E128" t="s">
+      <c r="E128" s="3" t="s">
         <v>253</v>
       </c>
-      <c r="F128" t="s">
+      <c r="F128" s="3" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="129" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E129" t="s">
+    <row r="129" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E129" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="F129" t="s">
+      <c r="F129" s="2" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="130" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="G129" s="2"/>
+    </row>
+    <row r="130" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E130" t="s">
         <v>257</v>
       </c>
@@ -17076,7 +17078,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="131" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="131" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E131" t="s">
         <v>259</v>
       </c>
@@ -17084,7 +17086,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="132" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="132" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E132" t="s">
         <v>261</v>
       </c>
@@ -17092,7 +17094,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="133" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="133" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E133" t="s">
         <v>263</v>
       </c>
@@ -17100,7 +17102,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="134" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="134" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E134" t="s">
         <v>265</v>
       </c>
@@ -17108,23 +17110,23 @@
         <v>266</v>
       </c>
     </row>
-    <row r="135" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E135" t="s">
+    <row r="135" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E135" s="2" t="s">
         <v>267</v>
       </c>
-      <c r="F135" t="s">
+      <c r="F135" s="2" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="136" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E136" t="s">
+    <row r="136" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E136" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="F136" t="s">
+      <c r="F136" s="2" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="137" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="137" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E137" t="s">
         <v>271</v>
       </c>
@@ -17132,7 +17134,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="138" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="138" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E138" t="s">
         <v>273</v>
       </c>
@@ -17140,7 +17142,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="139" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="139" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E139" t="s">
         <v>275</v>
       </c>
@@ -17148,7 +17150,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="140" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="140" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E140" t="s">
         <v>277</v>
       </c>
@@ -17156,15 +17158,15 @@
         <v>278</v>
       </c>
     </row>
-    <row r="141" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E141" t="s">
+    <row r="141" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E141" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="F141" t="s">
+      <c r="F141" s="2" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="142" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="142" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E142" t="s">
         <v>281</v>
       </c>
@@ -17172,7 +17174,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="143" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="143" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E143" t="s">
         <v>283</v>
       </c>
@@ -17180,7 +17182,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="144" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="144" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E144" t="s">
         <v>285</v>
       </c>
@@ -17188,7 +17190,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="145" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="145" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E145" t="s">
         <v>287</v>
       </c>
@@ -17196,7 +17198,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="146" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="146" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E146" t="s">
         <v>289</v>
       </c>
@@ -17204,7 +17206,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="147" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="147" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E147" t="s">
         <v>291</v>
       </c>
@@ -17212,7 +17214,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="148" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="148" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E148" t="s">
         <v>293</v>
       </c>
@@ -17220,7 +17222,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="149" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="149" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E149" t="s">
         <v>295</v>
       </c>
@@ -17228,7 +17230,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="150" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="150" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E150" t="s">
         <v>297</v>
       </c>
@@ -17236,31 +17238,32 @@
         <v>298</v>
       </c>
     </row>
-    <row r="151" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E151" t="s">
+    <row r="151" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E151" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="F151" t="s">
+      <c r="F151" s="2" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="152" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E152" t="s">
+    <row r="152" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E152" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="F152" t="s">
+      <c r="F152" s="2" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="153" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E153" t="s">
+    <row r="153" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E153" s="2" t="s">
         <v>303</v>
       </c>
-      <c r="F153" t="s">
+      <c r="F153" s="2" t="s">
         <v>304</v>
       </c>
-    </row>
-    <row r="154" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="G153" s="2"/>
+    </row>
+    <row r="154" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E154" t="s">
         <v>305</v>
       </c>
@@ -17268,7 +17271,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="155" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="155" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E155" t="s">
         <v>307</v>
       </c>
@@ -17276,7 +17279,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="156" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="156" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E156" t="s">
         <v>309</v>
       </c>
@@ -17284,7 +17287,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="157" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="157" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E157" t="s">
         <v>311</v>
       </c>
@@ -17294,18 +17297,23 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECA4C2FC-3D62-4498-96C6-3B296CB89802}">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:F5216"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21:D105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="46.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -58533,5 +58541,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>